<commit_message>
xModification to Excel database
TODO: rerender json file before final commit
</commit_message>
<xml_diff>
--- a/docs/IMDB Top 250 Movies.xlsx
+++ b/docs/IMDB Top 250 Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\react\movie-bucketlist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D0F73-5EFE-4F6B-8E75-F72D74E93B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3D4DED-DB66-4A9B-BAD8-6CF62C55B57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{346207D0-9AA0-42DB-A453-BB1282A9E7EA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="1087">
   <si>
     <t>Drama</t>
   </si>
@@ -3260,6 +3260,27 @@
   </si>
   <si>
     <t>topic</t>
+  </si>
+  <si>
+    <t>Comedy;Family</t>
+  </si>
+  <si>
+    <t>Home Alone</t>
+  </si>
+  <si>
+    <t>An eight-year-old troublemaker must protect his house from a pair of burglars when he is accidentally left home alone by his family during Christmas vacation.</t>
+  </si>
+  <si>
+    <t>Home Alone 2: Lost in New York</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>2h 00m</t>
+  </si>
+  <si>
+    <t>One year after Kevin McCallister was left home alone and had to defeat a pair of bumbling burglars, he accidentally finds himself stranded in New York City - and the same criminals are not far behind.</t>
   </si>
 </sst>
 </file>
@@ -4148,10 +4169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B372DD-848A-447C-BEE1-0C4F8EF77C63}">
-  <dimension ref="A1:K305"/>
+  <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14192,6 +14213,70 @@
       </c>
       <c r="K305" t="s">
         <v>1072</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A306">
+        <v>305</v>
+      </c>
+      <c r="B306">
+        <v>267</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E306" s="5">
+        <v>1990</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="H306" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="I306" t="s">
+        <v>906</v>
+      </c>
+      <c r="J306" t="s">
+        <v>322</v>
+      </c>
+      <c r="K306" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A307">
+        <v>306</v>
+      </c>
+      <c r="B307">
+        <v>267</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D307" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E307" s="5">
+        <v>1992</v>
+      </c>
+      <c r="F307" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="H307" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I307" t="s">
+        <v>906</v>
+      </c>
+      <c r="J307" t="s">
+        <v>1085</v>
+      </c>
+      <c r="K307" t="s">
+        <v>1086</v>
       </c>
     </row>
   </sheetData>
@@ -14211,7 +14296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H305">
+  <conditionalFormatting sqref="H2:H315">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>"8.0"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Change to spreadsheet: Harry Potter movie order was wrong
</commit_message>
<xml_diff>
--- a/docs/IMDB Top 250 Movies.xlsx
+++ b/docs/IMDB Top 250 Movies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\react\movie-bucketlist\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\react\movie-bucketlist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0728A3-D9E4-46ED-B014-6FE8DBA3F90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC854957-8508-4C0D-85E8-F647A4E95CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{346207D0-9AA0-42DB-A453-BB1282A9E7EA}"/>
   </bookViews>
@@ -4177,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B372DD-848A-447C-BEE1-0C4F8EF77C63}">
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K271" sqref="K271"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W96" sqref="W96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7010,26 +7010,26 @@
         <v>956</v>
       </c>
       <c r="D86" t="s">
-        <v>905</v>
+        <v>921</v>
       </c>
       <c r="E86" s="5">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="4" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="I86" t="s">
         <v>904</v>
       </c>
       <c r="J86" t="s">
-        <v>473</v>
+        <v>13</v>
       </c>
       <c r="K86" t="s">
-        <v>906</v>
+        <v>922</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
@@ -7043,26 +7043,26 @@
         <v>956</v>
       </c>
       <c r="D87" t="s">
-        <v>926</v>
+        <v>905</v>
       </c>
       <c r="E87" s="5">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="4" t="s">
-        <v>910</v>
+        <v>897</v>
       </c>
       <c r="I87" t="s">
-        <v>663</v>
+        <v>904</v>
       </c>
       <c r="J87" t="s">
-        <v>249</v>
+        <v>473</v>
       </c>
       <c r="K87" t="s">
-        <v>927</v>
+        <v>906</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
@@ -7076,26 +7076,26 @@
         <v>956</v>
       </c>
       <c r="D88" t="s">
-        <v>928</v>
+        <v>907</v>
       </c>
       <c r="E88" s="5">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="4" t="s">
-        <v>537</v>
+        <v>872</v>
       </c>
       <c r="I88" t="s">
-        <v>663</v>
+        <v>908</v>
       </c>
       <c r="J88" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="K88" t="s">
-        <v>664</v>
+        <v>923</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
@@ -7208,26 +7208,26 @@
         <v>956</v>
       </c>
       <c r="D92" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="E92" s="5">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="4" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="I92" t="s">
-        <v>904</v>
+        <v>663</v>
       </c>
       <c r="J92" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="K92" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
@@ -7241,26 +7241,26 @@
         <v>956</v>
       </c>
       <c r="D93" t="s">
-        <v>907</v>
+        <v>928</v>
       </c>
       <c r="E93" s="5">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="4" t="s">
-        <v>872</v>
+        <v>537</v>
       </c>
       <c r="I93" t="s">
-        <v>908</v>
+        <v>663</v>
       </c>
       <c r="J93" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="K93" t="s">
-        <v>923</v>
+        <v>664</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
@@ -14292,8 +14292,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K282">
-    <sortCondition ref="D199:D282"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K308">
+    <sortCondition ref="A67:A308"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">

</xml_diff>

<commit_message>
Changes to Spreadsheet Render new final CSV
</commit_message>
<xml_diff>
--- a/docs/IMDB Top 250 Movies.xlsx
+++ b/docs/IMDB Top 250 Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\react\movie-bucketlist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC854957-8508-4C0D-85E8-F647A4E95CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC953240-C93D-4725-ADD0-8FB26C357B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{346207D0-9AA0-42DB-A453-BB1282A9E7EA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="1101">
   <si>
     <t>Drama</t>
   </si>
@@ -3287,6 +3287,42 @@
   </si>
   <si>
     <t>Ex-Marine Tommy returns home and convinces his father to train him for a mixed martial arts tournament. However, there is more at stake than the prize money as he will be fighting against his brother.</t>
+  </si>
+  <si>
+    <t>deep-magenta</t>
+  </si>
+  <si>
+    <t>vibrant-blue</t>
+  </si>
+  <si>
+    <t>vivid-orange</t>
+  </si>
+  <si>
+    <t>vivid-green</t>
+  </si>
+  <si>
+    <t>bright-yellow</t>
+  </si>
+  <si>
+    <t>teal</t>
+  </si>
+  <si>
+    <t>electric-cyan</t>
+  </si>
+  <si>
+    <t>rich-indigo</t>
+  </si>
+  <si>
+    <t>lime-green</t>
+  </si>
+  <si>
+    <t>warm-coral</t>
+  </si>
+  <si>
+    <t>bright-red-orange</t>
+  </si>
+  <si>
+    <t>strong-purple</t>
   </si>
 </sst>
 </file>
@@ -3834,7 +3870,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3852,6 +3888,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4177,8 +4233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B372DD-848A-447C-BEE1-0C4F8EF77C63}">
   <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W96" sqref="W96"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D311" sqref="D311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4188,6 +4244,7 @@
     <col min="3" max="3" width="21.7265625" customWidth="1"/>
     <col min="4" max="4" width="47.7265625" customWidth="1"/>
     <col min="5" max="6" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" style="4"/>
     <col min="9" max="9" width="26.36328125" customWidth="1"/>
   </cols>
@@ -4477,7 +4534,9 @@
       <c r="F9" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>1089</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>380</v>
       </c>
@@ -4873,7 +4932,9 @@
       <c r="F21" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>1090</v>
+      </c>
       <c r="H21" s="4" t="s">
         <v>872</v>
       </c>
@@ -4906,7 +4967,9 @@
       <c r="F22" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>1090</v>
+      </c>
       <c r="H22" s="4" t="s">
         <v>866</v>
       </c>
@@ -5335,7 +5398,9 @@
       <c r="F35" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>1091</v>
+      </c>
       <c r="H35" s="4" t="s">
         <v>866</v>
       </c>
@@ -6358,7 +6423,9 @@
       <c r="F66" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G66" s="1"/>
+      <c r="G66" s="1" t="s">
+        <v>1091</v>
+      </c>
       <c r="H66" s="4" t="s">
         <v>537</v>
       </c>
@@ -6490,7 +6557,9 @@
       <c r="F70" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G70" s="1"/>
+      <c r="G70" s="1" t="s">
+        <v>1092</v>
+      </c>
       <c r="H70" s="4" t="s">
         <v>380</v>
       </c>
@@ -6556,7 +6625,9 @@
       <c r="F72" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>1093</v>
+      </c>
       <c r="H72" s="4" t="s">
         <v>121</v>
       </c>
@@ -6589,7 +6660,9 @@
       <c r="F73" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G73" s="1"/>
+      <c r="G73" s="1" t="s">
+        <v>1094</v>
+      </c>
       <c r="H73" s="4" t="s">
         <v>537</v>
       </c>
@@ -6655,7 +6728,9 @@
       <c r="F75" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G75" s="1"/>
+      <c r="G75" s="1" t="s">
+        <v>1095</v>
+      </c>
       <c r="H75" s="4" t="s">
         <v>261</v>
       </c>
@@ -6721,7 +6796,9 @@
       <c r="F77" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G77" s="1"/>
+      <c r="G77" s="1" t="s">
+        <v>1096</v>
+      </c>
       <c r="H77" s="4" t="s">
         <v>537</v>
       </c>
@@ -6787,7 +6864,9 @@
       <c r="F79" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G79" s="1"/>
+      <c r="G79" s="1" t="s">
+        <v>1095</v>
+      </c>
       <c r="H79" s="4" t="s">
         <v>380</v>
       </c>
@@ -6853,7 +6932,9 @@
       <c r="F81" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>1089</v>
+      </c>
       <c r="H81" s="4" t="s">
         <v>738</v>
       </c>
@@ -7810,7 +7891,9 @@
       <c r="F110" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G110" s="1"/>
+      <c r="G110" s="1" t="s">
+        <v>1097</v>
+      </c>
       <c r="H110" s="4" t="s">
         <v>537</v>
       </c>
@@ -7876,7 +7959,9 @@
       <c r="F112" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G112" s="1"/>
+      <c r="G112" s="1" t="s">
+        <v>1098</v>
+      </c>
       <c r="H112" s="4" t="s">
         <v>738</v>
       </c>
@@ -8140,7 +8225,9 @@
       <c r="F120" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G120" s="2"/>
+      <c r="G120" s="2" t="s">
+        <v>1093</v>
+      </c>
       <c r="H120" s="4" t="s">
         <v>380</v>
       </c>
@@ -8635,7 +8722,9 @@
       <c r="F135" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G135" s="1"/>
+      <c r="G135" s="1" t="s">
+        <v>1099</v>
+      </c>
       <c r="H135" s="4" t="s">
         <v>188</v>
       </c>
@@ -8833,7 +8922,9 @@
       <c r="F141" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G141" s="1"/>
+      <c r="G141" s="1" t="s">
+        <v>1089</v>
+      </c>
       <c r="H141" s="4" t="s">
         <v>380</v>
       </c>
@@ -8932,7 +9023,9 @@
       <c r="F144" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G144" s="1"/>
+      <c r="G144" s="1" t="s">
+        <v>1094</v>
+      </c>
       <c r="H144" s="4" t="s">
         <v>537</v>
       </c>
@@ -9196,7 +9289,9 @@
       <c r="F152" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G152" s="1"/>
+      <c r="G152" s="1" t="s">
+        <v>1090</v>
+      </c>
       <c r="H152" s="4" t="s">
         <v>75</v>
       </c>
@@ -9625,7 +9720,9 @@
       <c r="F165" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G165" s="1"/>
+      <c r="G165" s="1" t="s">
+        <v>1100</v>
+      </c>
       <c r="H165" s="4" t="s">
         <v>738</v>
       </c>
@@ -10054,7 +10151,9 @@
       <c r="F178" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G178" s="1"/>
+      <c r="G178" s="1" t="s">
+        <v>1089</v>
+      </c>
       <c r="H178" s="4" t="s">
         <v>20</v>
       </c>
@@ -10846,7 +10945,9 @@
       <c r="F202" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G202" s="1"/>
+      <c r="G202" s="1" t="s">
+        <v>1091</v>
+      </c>
       <c r="H202" s="4" t="s">
         <v>537</v>
       </c>
@@ -11800,7 +11901,9 @@
       <c r="F231" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G231" s="1"/>
+      <c r="G231" s="1" t="s">
+        <v>1094</v>
+      </c>
       <c r="H231" s="4" t="s">
         <v>39</v>
       </c>
@@ -11833,7 +11936,9 @@
       <c r="F232" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G232" s="1"/>
+      <c r="G232" s="1" t="s">
+        <v>1094</v>
+      </c>
       <c r="H232" s="4" t="s">
         <v>20</v>
       </c>
@@ -11866,7 +11971,9 @@
       <c r="F233" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G233" s="1"/>
+      <c r="G233" s="1" t="s">
+        <v>1094</v>
+      </c>
       <c r="H233" s="4" t="s">
         <v>51</v>
       </c>
@@ -11998,7 +12105,9 @@
       <c r="F237" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G237" s="1"/>
+      <c r="G237" s="1" t="s">
+        <v>1093</v>
+      </c>
       <c r="H237" s="4" t="s">
         <v>121</v>
       </c>
@@ -12394,7 +12503,9 @@
       <c r="F249" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G249" s="1"/>
+      <c r="G249" s="1" t="s">
+        <v>1090</v>
+      </c>
       <c r="H249" s="4" t="s">
         <v>380</v>
       </c>
@@ -12526,7 +12637,9 @@
       <c r="F253" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G253" s="1"/>
+      <c r="G253" s="1" t="s">
+        <v>1098</v>
+      </c>
       <c r="H253" s="4" t="s">
         <v>380</v>
       </c>
@@ -12592,7 +12705,9 @@
       <c r="F255" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G255" s="1"/>
+      <c r="G255" s="1" t="s">
+        <v>1099</v>
+      </c>
       <c r="H255" s="4" t="s">
         <v>537</v>
       </c>
@@ -12955,7 +13070,9 @@
       <c r="F266" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G266" s="1"/>
+      <c r="G266" s="1" t="s">
+        <v>1095</v>
+      </c>
       <c r="H266" s="4" t="s">
         <v>380</v>
       </c>
@@ -12988,7 +13105,9 @@
       <c r="F267" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="G267" s="1"/>
+      <c r="G267" s="1" t="s">
+        <v>1089</v>
+      </c>
       <c r="H267" s="4" t="s">
         <v>537</v>
       </c>
@@ -14296,8 +14415,16 @@
     <sortCondition ref="A67:A308"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="true">
+      <formula>NOT(ISERROR(SEARCH("true",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="false">
+      <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14309,14 +14436,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H315">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>"8.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
       <formula>"8.0"</formula>
       <formula>"7.5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
       <formula>"7.5"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Spreadsheet changes Reloaded database
</commit_message>
<xml_diff>
--- a/docs/IMDB Top 250 Movies.xlsx
+++ b/docs/IMDB Top 250 Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\react\movie-bucketlist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F73DAB0-7CFF-42E7-AF74-50E1D40C4EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA361CD9-DFF1-4B67-982F-CA9845FEB4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{346207D0-9AA0-42DB-A453-BB1282A9E7EA}"/>
   </bookViews>
@@ -3861,18 +3861,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4246,8 +4235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B372DD-848A-447C-BEE1-0C4F8EF77C63}">
   <dimension ref="A1:K306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F311" sqref="F311"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A250" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7392,26 +7381,26 @@
         <v>956</v>
       </c>
       <c r="D95" t="s">
-        <v>905</v>
+        <v>921</v>
       </c>
       <c r="E95" s="5">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="4" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="I95" t="s">
         <v>904</v>
       </c>
       <c r="J95" t="s">
-        <v>473</v>
+        <v>13</v>
       </c>
       <c r="K95" t="s">
-        <v>906</v>
+        <v>922</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
@@ -7425,26 +7414,26 @@
         <v>956</v>
       </c>
       <c r="D96" t="s">
-        <v>926</v>
+        <v>905</v>
       </c>
       <c r="E96" s="5">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="4" t="s">
-        <v>910</v>
+        <v>897</v>
       </c>
       <c r="I96" t="s">
-        <v>663</v>
+        <v>904</v>
       </c>
       <c r="J96" t="s">
-        <v>249</v>
+        <v>473</v>
       </c>
       <c r="K96" t="s">
-        <v>927</v>
+        <v>906</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
@@ -7458,26 +7447,26 @@
         <v>956</v>
       </c>
       <c r="D97" t="s">
-        <v>928</v>
+        <v>907</v>
       </c>
       <c r="E97" s="5">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="4" t="s">
-        <v>537</v>
+        <v>872</v>
       </c>
       <c r="I97" t="s">
-        <v>663</v>
+        <v>908</v>
       </c>
       <c r="J97" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="K97" t="s">
-        <v>664</v>
+        <v>923</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
@@ -7590,26 +7579,26 @@
         <v>956</v>
       </c>
       <c r="D101" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="E101" s="5">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="4" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="I101" t="s">
-        <v>904</v>
+        <v>663</v>
       </c>
       <c r="J101" t="s">
-        <v>13</v>
+        <v>249</v>
       </c>
       <c r="K101" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -7623,26 +7612,26 @@
         <v>956</v>
       </c>
       <c r="D102" t="s">
-        <v>907</v>
+        <v>928</v>
       </c>
       <c r="E102" s="5">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G102" s="2"/>
       <c r="H102" s="4" t="s">
-        <v>872</v>
+        <v>537</v>
       </c>
       <c r="I102" t="s">
-        <v>908</v>
+        <v>663</v>
       </c>
       <c r="J102" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="K102" t="s">
-        <v>923</v>
+        <v>664</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
@@ -8144,29 +8133,29 @@
         <v>97</v>
       </c>
       <c r="C118" t="s">
-        <v>449</v>
+        <v>224</v>
       </c>
       <c r="D118" t="s">
-        <v>931</v>
+        <v>225</v>
       </c>
       <c r="E118" s="5">
-        <v>2008</v>
+        <v>1981</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="G118" s="2"/>
+      <c r="G118" s="1"/>
       <c r="H118" s="4" t="s">
-        <v>932</v>
+        <v>188</v>
       </c>
       <c r="I118" t="s">
         <v>26</v>
       </c>
       <c r="J118" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="K118" t="s">
-        <v>933</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.35">
@@ -8180,26 +8169,26 @@
         <v>449</v>
       </c>
       <c r="D119" t="s">
-        <v>450</v>
+        <v>929</v>
       </c>
       <c r="E119" s="5">
-        <v>1989</v>
+        <v>1984</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="G119" s="1"/>
+      <c r="G119" s="2"/>
       <c r="H119" s="4" t="s">
-        <v>380</v>
+        <v>866</v>
       </c>
       <c r="I119" t="s">
         <v>26</v>
       </c>
       <c r="J119" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="K119" t="s">
-        <v>451</v>
+        <v>930</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.35">
@@ -8210,29 +8199,29 @@
         <v>97</v>
       </c>
       <c r="C120" t="s">
-        <v>224</v>
+        <v>449</v>
       </c>
       <c r="D120" t="s">
-        <v>225</v>
+        <v>450</v>
       </c>
       <c r="E120" s="5">
-        <v>1981</v>
+        <v>1989</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G120" s="1"/>
       <c r="H120" s="4" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
       <c r="I120" t="s">
         <v>26</v>
       </c>
       <c r="J120" t="s">
-        <v>226</v>
+        <v>81</v>
       </c>
       <c r="K120" t="s">
-        <v>227</v>
+        <v>451</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.35">
@@ -8246,26 +8235,26 @@
         <v>449</v>
       </c>
       <c r="D121" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="E121" s="5">
-        <v>1984</v>
+        <v>2008</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>864</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="4" t="s">
-        <v>866</v>
+        <v>932</v>
       </c>
       <c r="I121" t="s">
         <v>26</v>
       </c>
       <c r="J121" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="K121" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.35">
@@ -12805,10 +12794,10 @@
         <v>29</v>
       </c>
       <c r="D259" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E259" s="5">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>881</v>
@@ -12817,16 +12806,16 @@
         <v>1091</v>
       </c>
       <c r="H259" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="I259" t="s">
         <v>31</v>
       </c>
       <c r="J259" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="K259" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.35">
@@ -12840,10 +12829,10 @@
         <v>29</v>
       </c>
       <c r="D260" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="E260" s="5">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>881</v>
@@ -12852,16 +12841,16 @@
         <v>1091</v>
       </c>
       <c r="H260" s="4" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="I260" t="s">
         <v>31</v>
       </c>
       <c r="J260" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="K260" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.35">
@@ -14400,15 +14389,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K306">
-    <sortCondition ref="D1:D306"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K308">
+    <sortCondition ref="A250:A308"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="true">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH("true",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="false">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14425,19 +14417,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H314">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>"8.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
       <formula>"8.0"</formula>
       <formula>"7.5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>"7.5"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Soft Hyphen fix for Blackkklansman
</commit_message>
<xml_diff>
--- a/docs/IMDB Top 250 Movies.xlsx
+++ b/docs/IMDB Top 250 Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\react\movie-bucketlist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA361CD9-DFF1-4B67-982F-CA9845FEB4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911E819F-41A5-4A31-A077-68BDF752BF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{346207D0-9AA0-42DB-A453-BB1282A9E7EA}"/>
   </bookViews>
@@ -2617,9 +2617,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>BlacKkKlansman</t>
-  </si>
-  <si>
     <t>7.5</t>
   </si>
   <si>
@@ -3314,6 +3311,9 @@
   </si>
   <si>
     <t>strong-purple</t>
+  </si>
+  <si>
+    <t>BlacKkKlans­man</t>
   </si>
 </sst>
 </file>
@@ -4235,8 +4235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B372DD-848A-447C-BEE1-0C4F8EF77C63}">
   <dimension ref="A1:K306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A250" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4253,37 +4253,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1" t="s">
         <v>1068</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>891</v>
+      </c>
+      <c r="D1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="C1" t="s">
-        <v>892</v>
-      </c>
-      <c r="D1" t="s">
-        <v>891</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" t="s">
         <v>893</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="I1" t="s">
         <v>1070</v>
       </c>
-      <c r="G1" t="s">
-        <v>894</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" t="s">
         <v>1072</v>
       </c>
-      <c r="I1" t="s">
-        <v>1071</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1073</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I4" t="s">
         <v>782</v>
@@ -4382,7 +4382,7 @@
         <v>210</v>
       </c>
       <c r="K4" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -4534,10 +4534,10 @@
         <v>1971</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>380</v>
@@ -4593,10 +4593,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D11" t="s">
         <v>1010</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1011</v>
       </c>
       <c r="E11">
         <v>1988</v>
@@ -4608,13 +4608,13 @@
         <v>738</v>
       </c>
       <c r="I11" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="J11" t="s">
         <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -4955,22 +4955,22 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
+        <v>869</v>
+      </c>
+      <c r="D22" t="s">
         <v>870</v>
-      </c>
-      <c r="D22" t="s">
-        <v>871</v>
       </c>
       <c r="E22" s="5">
         <v>2009</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I22" t="s">
         <v>122</v>
@@ -4979,7 +4979,7 @@
         <v>504</v>
       </c>
       <c r="K22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -4990,31 +4990,31 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D23" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E23" s="5">
         <v>2022</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I23" t="s">
         <v>122</v>
       </c>
       <c r="J23" t="s">
+        <v>874</v>
+      </c>
+      <c r="K23" t="s">
         <v>875</v>
-      </c>
-      <c r="K23" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -5091,7 +5091,7 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D26" t="s">
         <v>124</v>
@@ -5113,7 +5113,7 @@
         <v>108</v>
       </c>
       <c r="K26" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -5124,10 +5124,10 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D27" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E27" s="5">
         <v>1989</v>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I27" t="s">
         <v>48</v>
@@ -5146,7 +5146,7 @@
         <v>348</v>
       </c>
       <c r="K27" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -5157,10 +5157,10 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D28" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E28" s="5">
         <v>1990</v>
@@ -5170,7 +5170,7 @@
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I28" t="s">
         <v>48</v>
@@ -5179,7 +5179,7 @@
         <v>96</v>
       </c>
       <c r="K28" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -5421,31 +5421,31 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D36" t="s">
-        <v>865</v>
+        <v>1097</v>
       </c>
       <c r="E36" s="5">
         <v>2018</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="H36" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="I36" t="s">
         <v>866</v>
-      </c>
-      <c r="I36" t="s">
-        <v>867</v>
       </c>
       <c r="J36" t="s">
         <v>525</v>
       </c>
       <c r="K36" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -5555,10 +5555,10 @@
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D40" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E40">
         <v>1976</v>
@@ -5567,7 +5567,7 @@
         <v>864</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I40" t="s">
         <v>403</v>
@@ -5576,7 +5576,7 @@
         <v>234</v>
       </c>
       <c r="K40" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -6151,7 +6151,7 @@
         <v>442</v>
       </c>
       <c r="D58" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E58" s="5">
         <v>1990</v>
@@ -6161,16 +6161,16 @@
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="I58" t="s">
         <v>898</v>
-      </c>
-      <c r="I58" t="s">
-        <v>899</v>
       </c>
       <c r="J58" t="s">
         <v>65</v>
       </c>
       <c r="K58" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
@@ -6184,7 +6184,7 @@
         <v>442</v>
       </c>
       <c r="D59" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E59" s="5">
         <v>1995</v>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I59" t="s">
         <v>444</v>
@@ -6203,7 +6203,7 @@
         <v>381</v>
       </c>
       <c r="K59" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
@@ -6247,10 +6247,10 @@
         <v>51</v>
       </c>
       <c r="C61" t="s">
+        <v>997</v>
+      </c>
+      <c r="D61" t="s">
         <v>998</v>
-      </c>
-      <c r="D61" t="s">
-        <v>999</v>
       </c>
       <c r="E61">
         <v>2001</v>
@@ -6262,13 +6262,13 @@
         <v>738</v>
       </c>
       <c r="I61" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="J61" t="s">
         <v>218</v>
       </c>
       <c r="K61" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
@@ -6348,7 +6348,7 @@
         <v>267</v>
       </c>
       <c r="D64" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E64" s="5">
         <v>1964</v>
@@ -6367,7 +6367,7 @@
         <v>268</v>
       </c>
       <c r="K64" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
@@ -6378,10 +6378,10 @@
         <v>55</v>
       </c>
       <c r="C65" t="s">
+        <v>984</v>
+      </c>
+      <c r="D65" t="s">
         <v>985</v>
-      </c>
-      <c r="D65" t="s">
-        <v>986</v>
       </c>
       <c r="E65">
         <v>2011</v>
@@ -6390,16 +6390,16 @@
         <v>864</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I65" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="J65" t="s">
         <v>561</v>
       </c>
       <c r="K65" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
@@ -6410,10 +6410,10 @@
         <v>56</v>
       </c>
       <c r="C66" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D66" t="s">
         <v>1025</v>
-      </c>
-      <c r="D66" t="s">
-        <v>1026</v>
       </c>
       <c r="E66">
         <v>2021</v>
@@ -6431,7 +6431,7 @@
         <v>154</v>
       </c>
       <c r="K66" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
@@ -6442,10 +6442,10 @@
         <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D67" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E67">
         <v>2024</v>
@@ -6460,10 +6460,10 @@
         <v>447</v>
       </c>
       <c r="J67" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="K67" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
@@ -6474,10 +6474,10 @@
         <v>57</v>
       </c>
       <c r="C68" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D68" t="s">
         <v>1018</v>
-      </c>
-      <c r="D68" t="s">
-        <v>1019</v>
       </c>
       <c r="E68">
         <v>1990</v>
@@ -6486,16 +6486,16 @@
         <v>864</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I68" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="J68" t="s">
         <v>294</v>
       </c>
       <c r="K68" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
@@ -6572,10 +6572,10 @@
         <v>60</v>
       </c>
       <c r="C71" t="s">
+        <v>987</v>
+      </c>
+      <c r="D71" t="s">
         <v>988</v>
-      </c>
-      <c r="D71" t="s">
-        <v>989</v>
       </c>
       <c r="E71">
         <v>2014</v>
@@ -6584,16 +6584,16 @@
         <v>864</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I71" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="J71" t="s">
         <v>348</v>
       </c>
       <c r="K71" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
@@ -6679,10 +6679,10 @@
         <v>2003</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>537</v>
@@ -6813,10 +6813,10 @@
         <v>1987</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>380</v>
@@ -6872,10 +6872,10 @@
         <v>69</v>
       </c>
       <c r="C80" t="s">
+        <v>976</v>
+      </c>
+      <c r="D80" t="s">
         <v>977</v>
-      </c>
-      <c r="D80" t="s">
-        <v>978</v>
       </c>
       <c r="E80">
         <v>2017</v>
@@ -6884,16 +6884,16 @@
         <v>864</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I80" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="J80" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="K80" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
@@ -6913,10 +6913,10 @@
         <v>2000</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>121</v>
@@ -6948,10 +6948,10 @@
         <v>2014</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>537</v>
@@ -7016,10 +7016,10 @@
         <v>1997</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>261</v>
@@ -7084,10 +7084,10 @@
         <v>2008</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>537</v>
@@ -7152,10 +7152,10 @@
         <v>2018</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>380</v>
@@ -7211,31 +7211,31 @@
         <v>79</v>
       </c>
       <c r="C90" t="s">
+        <v>876</v>
+      </c>
+      <c r="D90" t="s">
         <v>877</v>
-      </c>
-      <c r="D90" t="s">
-        <v>878</v>
       </c>
       <c r="E90" s="5">
         <v>2014</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>738</v>
       </c>
       <c r="I90" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="J90" t="s">
         <v>118</v>
       </c>
       <c r="K90" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
@@ -7378,10 +7378,10 @@
         <v>84</v>
       </c>
       <c r="C95" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D95" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E95" s="5">
         <v>2001</v>
@@ -7391,16 +7391,16 @@
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I95" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J95" t="s">
         <v>13</v>
       </c>
       <c r="K95" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
@@ -7411,10 +7411,10 @@
         <v>84</v>
       </c>
       <c r="C96" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D96" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E96" s="5">
         <v>2002</v>
@@ -7424,16 +7424,16 @@
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I96" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J96" t="s">
         <v>473</v>
       </c>
       <c r="K96" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
@@ -7444,10 +7444,10 @@
         <v>84</v>
       </c>
       <c r="C97" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D97" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E97" s="5">
         <v>2004</v>
@@ -7457,16 +7457,16 @@
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I97" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J97" t="s">
         <v>4</v>
       </c>
       <c r="K97" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
@@ -7477,10 +7477,10 @@
         <v>84</v>
       </c>
       <c r="C98" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D98" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E98" s="5">
         <v>2005</v>
@@ -7490,16 +7490,16 @@
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="I98" t="s">
         <v>910</v>
       </c>
-      <c r="I98" t="s">
+      <c r="J98" t="s">
         <v>911</v>
       </c>
-      <c r="J98" t="s">
-        <v>912</v>
-      </c>
       <c r="K98" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
@@ -7510,10 +7510,10 @@
         <v>84</v>
       </c>
       <c r="C99" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D99" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E99" s="5">
         <v>2009</v>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I99" t="s">
         <v>663</v>
@@ -7532,7 +7532,7 @@
         <v>36</v>
       </c>
       <c r="K99" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
@@ -7543,10 +7543,10 @@
         <v>84</v>
       </c>
       <c r="C100" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D100" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E100" s="5">
         <v>2007</v>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="G100" s="2"/>
       <c r="H100" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I100" t="s">
         <v>663</v>
@@ -7565,7 +7565,7 @@
         <v>420</v>
       </c>
       <c r="K100" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
@@ -7576,10 +7576,10 @@
         <v>84</v>
       </c>
       <c r="C101" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D101" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E101" s="5">
         <v>2010</v>
@@ -7589,7 +7589,7 @@
       </c>
       <c r="G101" s="2"/>
       <c r="H101" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I101" t="s">
         <v>663</v>
@@ -7598,7 +7598,7 @@
         <v>249</v>
       </c>
       <c r="K101" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
@@ -7609,10 +7609,10 @@
         <v>84</v>
       </c>
       <c r="C102" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D102" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E102" s="5">
         <v>2011</v>
@@ -7675,10 +7675,10 @@
         <v>86</v>
       </c>
       <c r="C104" t="s">
+        <v>968</v>
+      </c>
+      <c r="D104" t="s">
         <v>969</v>
-      </c>
-      <c r="D104" t="s">
-        <v>970</v>
       </c>
       <c r="E104">
         <v>2018</v>
@@ -7687,16 +7687,16 @@
         <v>864</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I104" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J104" t="s">
         <v>81</v>
       </c>
       <c r="K104" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
@@ -7740,10 +7740,10 @@
         <v>88</v>
       </c>
       <c r="C106" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D106" t="s">
         <v>1075</v>
-      </c>
-      <c r="D106" t="s">
-        <v>1076</v>
       </c>
       <c r="E106" s="5">
         <v>1990</v>
@@ -7752,16 +7752,16 @@
         <v>864</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I106" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J106" t="s">
         <v>320</v>
       </c>
       <c r="K106" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.35">
@@ -7772,10 +7772,10 @@
         <v>88</v>
       </c>
       <c r="C107" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D107" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E107" s="5">
         <v>1992</v>
@@ -7784,16 +7784,16 @@
         <v>864</v>
       </c>
       <c r="H107" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I107" t="s">
+        <v>903</v>
+      </c>
+      <c r="J107" t="s">
         <v>1079</v>
       </c>
-      <c r="I107" t="s">
-        <v>904</v>
-      </c>
-      <c r="J107" t="s">
+      <c r="K107" t="s">
         <v>1080</v>
-      </c>
-      <c r="K107" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.35">
@@ -7837,7 +7837,7 @@
         <v>90</v>
       </c>
       <c r="C109" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>713</v>
@@ -7853,7 +7853,7 @@
         <v>537</v>
       </c>
       <c r="I109" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J109" t="s">
         <v>234</v>
@@ -7870,10 +7870,10 @@
         <v>90</v>
       </c>
       <c r="C110" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E110" s="1">
         <v>2014</v>
@@ -7883,16 +7883,16 @@
       </c>
       <c r="G110" s="2"/>
       <c r="H110" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I110" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J110" t="s">
         <v>173</v>
       </c>
       <c r="K110" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
@@ -7903,10 +7903,10 @@
         <v>90</v>
       </c>
       <c r="C111" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E111" s="1">
         <v>2019</v>
@@ -7916,16 +7916,16 @@
       </c>
       <c r="G111" s="2"/>
       <c r="H111" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I111" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J111" t="s">
+        <v>965</v>
+      </c>
+      <c r="K111" t="s">
         <v>966</v>
-      </c>
-      <c r="K111" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.35">
@@ -8005,7 +8005,7 @@
         <v>46</v>
       </c>
       <c r="D114" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E114">
         <v>2000</v>
@@ -8017,13 +8017,13 @@
         <v>537</v>
       </c>
       <c r="I114" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="J114" t="s">
         <v>234</v>
       </c>
       <c r="K114" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.35">
@@ -8169,7 +8169,7 @@
         <v>449</v>
       </c>
       <c r="D119" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E119" s="5">
         <v>1984</v>
@@ -8179,7 +8179,7 @@
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I119" t="s">
         <v>26</v>
@@ -8188,7 +8188,7 @@
         <v>96</v>
       </c>
       <c r="K119" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.35">
@@ -8235,7 +8235,7 @@
         <v>449</v>
       </c>
       <c r="D121" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E121" s="5">
         <v>2008</v>
@@ -8245,7 +8245,7 @@
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I121" t="s">
         <v>26</v>
@@ -8254,7 +8254,7 @@
         <v>265</v>
       </c>
       <c r="K121" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.35">
@@ -8307,10 +8307,10 @@
         <v>2015</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="H123" s="4" t="s">
         <v>537</v>
@@ -8375,10 +8375,10 @@
         <v>2007</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="H125" s="4" t="s">
         <v>738</v>
@@ -8621,7 +8621,7 @@
         <v>81</v>
       </c>
       <c r="K132" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.35">
@@ -8632,7 +8632,7 @@
         <v>109</v>
       </c>
       <c r="C133" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D133" t="s">
         <v>553</v>
@@ -8641,10 +8641,10 @@
         <v>2003</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H133" s="4" t="s">
         <v>380</v>
@@ -8667,10 +8667,10 @@
         <v>109</v>
       </c>
       <c r="C134" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D134" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E134" s="5">
         <v>2004</v>
@@ -8689,7 +8689,7 @@
         <v>123</v>
       </c>
       <c r="K134" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.35">
@@ -8700,10 +8700,10 @@
         <v>110</v>
       </c>
       <c r="C135" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D135" t="s">
         <v>1034</v>
-      </c>
-      <c r="D135" t="s">
-        <v>1035</v>
       </c>
       <c r="E135">
         <v>2023</v>
@@ -8712,16 +8712,16 @@
         <v>864</v>
       </c>
       <c r="H135" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I135" t="s">
         <v>71</v>
       </c>
       <c r="J135" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="K135" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.35">
@@ -8831,10 +8831,10 @@
         <v>114</v>
       </c>
       <c r="C139" t="s">
+        <v>979</v>
+      </c>
+      <c r="D139" t="s">
         <v>980</v>
-      </c>
-      <c r="D139" t="s">
-        <v>981</v>
       </c>
       <c r="E139">
         <v>2017</v>
@@ -8843,16 +8843,16 @@
         <v>864</v>
       </c>
       <c r="H139" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I139" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="J139" t="s">
         <v>829</v>
       </c>
       <c r="K139" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.35">
@@ -9094,10 +9094,10 @@
         <v>122</v>
       </c>
       <c r="C147" t="s">
+        <v>990</v>
+      </c>
+      <c r="D147" t="s">
         <v>991</v>
-      </c>
-      <c r="D147" t="s">
-        <v>992</v>
       </c>
       <c r="E147">
         <v>2003</v>
@@ -9106,16 +9106,16 @@
         <v>864</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I147" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="J147" t="s">
         <v>173</v>
       </c>
       <c r="K147" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.35">
@@ -9234,10 +9234,10 @@
         <v>2000</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="H151" s="4" t="s">
         <v>188</v>
@@ -9326,10 +9326,10 @@
         <v>129</v>
       </c>
       <c r="C154" t="s">
+        <v>974</v>
+      </c>
+      <c r="D154" t="s">
         <v>975</v>
-      </c>
-      <c r="D154" t="s">
-        <v>976</v>
       </c>
       <c r="E154">
         <v>2019</v>
@@ -9338,16 +9338,16 @@
         <v>864</v>
       </c>
       <c r="H154" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I154" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J154" t="s">
         <v>57</v>
       </c>
       <c r="K154" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.35">
@@ -9466,10 +9466,10 @@
         <v>1975</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H158" s="4" t="s">
         <v>380</v>
@@ -9495,7 +9495,7 @@
         <v>46</v>
       </c>
       <c r="D159" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E159">
         <v>2016</v>
@@ -9504,16 +9504,16 @@
         <v>864</v>
       </c>
       <c r="H159" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I159" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="J159" t="s">
         <v>554</v>
       </c>
       <c r="K159" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.35">
@@ -9557,10 +9557,10 @@
         <v>136</v>
       </c>
       <c r="C161" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D161" t="s">
         <v>1001</v>
-      </c>
-      <c r="D161" t="s">
-        <v>1002</v>
       </c>
       <c r="E161">
         <v>2001</v>
@@ -9569,16 +9569,16 @@
         <v>864</v>
       </c>
       <c r="H161" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I161" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="J161" t="s">
         <v>222</v>
       </c>
       <c r="K161" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.35">
@@ -9631,10 +9631,10 @@
         <v>1988</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H163" s="4" t="s">
         <v>537</v>
@@ -9690,10 +9690,10 @@
         <v>140</v>
       </c>
       <c r="C165" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D165" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E165">
         <v>1968</v>
@@ -9702,16 +9702,16 @@
         <v>864</v>
       </c>
       <c r="H165" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I165" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="J165" t="s">
         <v>22</v>
       </c>
       <c r="K165" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.35">
@@ -9929,10 +9929,10 @@
         <v>1975</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H172" s="4" t="s">
         <v>75</v>
@@ -9977,7 +9977,7 @@
         <v>96</v>
       </c>
       <c r="K173" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.35">
@@ -10024,7 +10024,7 @@
         <v>247</v>
       </c>
       <c r="D175" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E175">
         <v>2023</v>
@@ -10033,16 +10033,16 @@
         <v>864</v>
       </c>
       <c r="H175" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I175" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="J175" t="s">
         <v>294</v>
       </c>
       <c r="K175" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.35">
@@ -10174,7 +10174,7 @@
         <v>354</v>
       </c>
       <c r="K179" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.35">
@@ -10218,10 +10218,10 @@
         <v>156</v>
       </c>
       <c r="C181" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D181" t="s">
         <v>1004</v>
-      </c>
-      <c r="D181" t="s">
-        <v>1005</v>
       </c>
       <c r="E181">
         <v>2023</v>
@@ -10233,13 +10233,13 @@
         <v>188</v>
       </c>
       <c r="I181" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="J181" t="s">
         <v>630</v>
       </c>
       <c r="K181" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.35">
@@ -10424,10 +10424,10 @@
         <v>1988</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H187" s="4" t="s">
         <v>738</v>
@@ -10780,10 +10780,10 @@
         <v>173</v>
       </c>
       <c r="C198" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D198" t="s">
         <v>1007</v>
-      </c>
-      <c r="D198" t="s">
-        <v>1008</v>
       </c>
       <c r="E198">
         <v>2023</v>
@@ -10792,16 +10792,16 @@
         <v>864</v>
       </c>
       <c r="H198" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I198" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="J198" t="s">
         <v>81</v>
       </c>
       <c r="K198" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.35">
@@ -10887,10 +10887,10 @@
         <v>1993</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H201" s="4" t="s">
         <v>20</v>
@@ -11213,7 +11213,7 @@
         <v>62</v>
       </c>
       <c r="D211" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E211" s="5">
         <v>1999</v>
@@ -11223,7 +11223,7 @@
       </c>
       <c r="G211" s="2"/>
       <c r="H211" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I211" t="s">
         <v>117</v>
@@ -11232,7 +11232,7 @@
         <v>68</v>
       </c>
       <c r="K211" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.35">
@@ -11246,7 +11246,7 @@
         <v>62</v>
       </c>
       <c r="D212" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E212" s="5">
         <v>2002</v>
@@ -11256,7 +11256,7 @@
       </c>
       <c r="G212" s="2"/>
       <c r="H212" s="4" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I212" t="s">
         <v>117</v>
@@ -11265,7 +11265,7 @@
         <v>4</v>
       </c>
       <c r="K212" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.35">
@@ -11279,7 +11279,7 @@
         <v>62</v>
       </c>
       <c r="D213" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E213" s="5">
         <v>2005</v>
@@ -11289,7 +11289,7 @@
       </c>
       <c r="G213" s="2"/>
       <c r="H213" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I213" t="s">
         <v>117</v>
@@ -11298,7 +11298,7 @@
         <v>468</v>
       </c>
       <c r="K213" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.35">
@@ -11312,7 +11312,7 @@
         <v>62</v>
       </c>
       <c r="D214" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E214" s="5">
         <v>1977</v>
@@ -11364,7 +11364,7 @@
         <v>65</v>
       </c>
       <c r="K215" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.35">
@@ -11441,10 +11441,10 @@
         <v>188</v>
       </c>
       <c r="C218" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D218" t="s">
         <v>1029</v>
-      </c>
-      <c r="D218" t="s">
-        <v>1030</v>
       </c>
       <c r="E218">
         <v>2023</v>
@@ -11453,16 +11453,16 @@
         <v>864</v>
       </c>
       <c r="H218" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I218" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="J218" t="s">
         <v>268</v>
       </c>
       <c r="K218" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.35">
@@ -11509,7 +11509,7 @@
         <v>66</v>
       </c>
       <c r="D220" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E220" s="5">
         <v>1984</v>
@@ -11561,7 +11561,7 @@
         <v>123</v>
       </c>
       <c r="K221" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.35">
@@ -11713,10 +11713,10 @@
         <v>1998</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="H226" s="4" t="s">
         <v>537</v>
@@ -11772,10 +11772,10 @@
         <v>197</v>
       </c>
       <c r="C228" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D228" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E228">
         <v>1985</v>
@@ -11784,16 +11784,16 @@
         <v>864</v>
       </c>
       <c r="H228" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I228" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="J228" t="s">
         <v>484</v>
       </c>
       <c r="K228" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.35">
@@ -11837,7 +11837,7 @@
         <v>199</v>
       </c>
       <c r="C230" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D230" t="s">
         <v>10</v>
@@ -11870,7 +11870,7 @@
         <v>199</v>
       </c>
       <c r="C231" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D231" t="s">
         <v>270</v>
@@ -11999,10 +11999,10 @@
         <v>203</v>
       </c>
       <c r="C235" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D235" t="s">
         <v>1015</v>
-      </c>
-      <c r="D235" t="s">
-        <v>1016</v>
       </c>
       <c r="E235">
         <v>1981</v>
@@ -12011,16 +12011,16 @@
         <v>864</v>
       </c>
       <c r="H235" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I235" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="J235" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="K235" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.35">
@@ -12130,7 +12130,7 @@
         <v>207</v>
       </c>
       <c r="C239" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D239" t="s">
         <v>6</v>
@@ -12152,7 +12152,7 @@
         <v>8</v>
       </c>
       <c r="K239" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.35">
@@ -12163,7 +12163,7 @@
         <v>207</v>
       </c>
       <c r="C240" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D240" t="s">
         <v>16</v>
@@ -12196,10 +12196,10 @@
         <v>207</v>
       </c>
       <c r="C241" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D241" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E241" s="5">
         <v>1990</v>
@@ -12209,7 +12209,7 @@
       </c>
       <c r="G241" s="2"/>
       <c r="H241" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I241" t="s">
         <v>7</v>
@@ -12218,7 +12218,7 @@
         <v>504</v>
       </c>
       <c r="K241" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.35">
@@ -12658,10 +12658,10 @@
         <v>221</v>
       </c>
       <c r="C255" t="s">
+        <v>971</v>
+      </c>
+      <c r="D255" t="s">
         <v>972</v>
-      </c>
-      <c r="D255" t="s">
-        <v>973</v>
       </c>
       <c r="E255">
         <v>2019</v>
@@ -12670,16 +12670,16 @@
         <v>864</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I255" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="J255" t="s">
         <v>131</v>
       </c>
       <c r="K255" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.35">
@@ -12765,10 +12765,10 @@
         <v>2001</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H258" s="4" t="s">
         <v>39</v>
@@ -12800,10 +12800,10 @@
         <v>2002</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H259" s="4" t="s">
         <v>51</v>
@@ -12835,10 +12835,10 @@
         <v>2003</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H260" s="4" t="s">
         <v>20</v>
@@ -12877,13 +12877,13 @@
         <v>51</v>
       </c>
       <c r="I261" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="J261" t="s">
         <v>68</v>
       </c>
       <c r="K261" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.35">
@@ -12897,7 +12897,7 @@
         <v>698</v>
       </c>
       <c r="D262" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E262">
         <v>2022</v>
@@ -12906,16 +12906,16 @@
         <v>864</v>
       </c>
       <c r="H262" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I262" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="J262" t="s">
         <v>398</v>
       </c>
       <c r="K262" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.35">
@@ -13001,10 +13001,10 @@
         <v>2006</v>
       </c>
       <c r="F265" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="H265" s="4" t="s">
         <v>121</v>
@@ -13027,10 +13027,10 @@
         <v>230</v>
       </c>
       <c r="C266" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D266" t="s">
         <v>1022</v>
-      </c>
-      <c r="D266" t="s">
-        <v>1023</v>
       </c>
       <c r="E266">
         <v>1975</v>
@@ -13039,16 +13039,16 @@
         <v>864</v>
       </c>
       <c r="H266" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I266" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="J266" t="s">
         <v>561</v>
       </c>
       <c r="K266" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.35">
@@ -13431,10 +13431,10 @@
         <v>1998</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H278" s="4" t="s">
         <v>380</v>
@@ -13526,7 +13526,7 @@
         <v>698</v>
       </c>
       <c r="D281" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="E281">
         <v>2022</v>
@@ -13535,7 +13535,7 @@
         <v>864</v>
       </c>
       <c r="H281" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I281" t="s">
         <v>323</v>
@@ -13544,7 +13544,7 @@
         <v>210</v>
       </c>
       <c r="K281" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.35">
@@ -13597,10 +13597,10 @@
         <v>2013</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="H283" s="4" t="s">
         <v>380</v>
@@ -13665,10 +13665,10 @@
         <v>2017</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="H285" s="4" t="s">
         <v>537</v>
@@ -13823,7 +13823,7 @@
         <v>254</v>
       </c>
       <c r="C290" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D290" t="s">
         <v>288</v>
@@ -13832,10 +13832,10 @@
         <v>1995</v>
       </c>
       <c r="F290" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H290" s="4" t="s">
         <v>261</v>
@@ -13858,22 +13858,22 @@
         <v>254</v>
       </c>
       <c r="C291" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D291" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E291" s="5">
         <v>1999</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H291" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I291" t="s">
         <v>289</v>
@@ -13882,7 +13882,7 @@
         <v>718</v>
       </c>
       <c r="K291" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.35">
@@ -13893,7 +13893,7 @@
         <v>254</v>
       </c>
       <c r="C292" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D292" t="s">
         <v>318</v>
@@ -13902,10 +13902,10 @@
         <v>2010</v>
       </c>
       <c r="F292" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H292" s="4" t="s">
         <v>261</v>
@@ -13928,31 +13928,31 @@
         <v>254</v>
       </c>
       <c r="C293" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D293" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E293" s="5">
         <v>2019</v>
       </c>
       <c r="F293" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="H293" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I293" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="J293" t="s">
         <v>561</v>
       </c>
       <c r="K293" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.35">
@@ -14038,10 +14038,10 @@
         <v>2009</v>
       </c>
       <c r="F296" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="H296" s="4" t="s">
         <v>380</v>
@@ -14073,10 +14073,10 @@
         <v>2005</v>
       </c>
       <c r="F297" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H297" s="4" t="s">
         <v>537</v>
@@ -14187,7 +14187,7 @@
         <v>468</v>
       </c>
       <c r="K300" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>